<commit_message>
Corrección de columnas en matriz de excel
</commit_message>
<xml_diff>
--- a/FW/Matriz y Conexiones.xlsx
+++ b/FW/Matriz y Conexiones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://isiamadness-my.sharepoint.com/personal/adrian_clz20_isiamadness_onmicrosoft_com/Documents/Documentos/GitHub/narfkb2/FW/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{DFD1DFD2-98CC-49AC-9ACC-905A4F1A9B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B3AC778-E47B-47B5-BF8D-2CE8CC52B754}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="8_{DFD1DFD2-98CC-49AC-9ACC-905A4F1A9B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3BE73E3-C7F2-40D7-9113-C3CA0CA66F8F}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-132" windowWidth="23256" windowHeight="12456" xr2:uid="{8D32C868-F4C7-4A29-AE88-EBB6DC122651}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
   <si>
     <t>C1</t>
   </si>
@@ -65,18 +65,12 @@
     <t>R3</t>
   </si>
   <si>
-    <t>R4</t>
-  </si>
-  <si>
     <t>C7</t>
   </si>
   <si>
     <t>C8</t>
   </si>
   <si>
-    <t>C9</t>
-  </si>
-  <si>
     <t>RX</t>
   </si>
   <si>
@@ -156,13 +150,22 @@
   </si>
   <si>
     <t>Controlador Derecho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C0 </t>
+  </si>
+  <si>
+    <t>R0</t>
+  </si>
+  <si>
+    <t>C0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,6 +210,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -234,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -252,12 +263,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -266,6 +271,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DE72ECA-C84D-4A81-8463-48A3DE568D4E}">
   <dimension ref="A1:W18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,376 +613,376 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C1" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
+      <c r="C1" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="10"/>
+      <c r="M2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="12"/>
-      <c r="M2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="O2" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="P2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="R2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="T2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="U2" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="E3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="F3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="G3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="H3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="I3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="J3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="L3" s="12"/>
-      <c r="M3" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="O3" s="9" t="s">
+      <c r="L3" s="10"/>
+      <c r="M3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="9" t="s">
+      <c r="N3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="O3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" s="9" t="s">
+      <c r="P3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="R3" s="9" t="s">
+      <c r="Q3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="S3" s="9" t="s">
+      <c r="R3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="T3" s="9" t="s">
+      <c r="S3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="U3" s="9" t="s">
+      <c r="T3" s="7" t="s">
         <v>0</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="C4" s="2" t="str">
         <f>_xlfn.CONCAT( C3,",",$B$4)</f>
-        <v>C1,R1</v>
+        <v>C0,R0</v>
       </c>
       <c r="D4" s="2" t="str">
         <f t="shared" ref="D4:H4" si="0">_xlfn.CONCAT( D3,",",$B$4)</f>
-        <v>C2,R1</v>
+        <v>C1,R0</v>
       </c>
       <c r="E4" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>C3,R1</v>
+        <v>C2,R0</v>
       </c>
       <c r="F4" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>C4,R1</v>
+        <v>C3,R0</v>
       </c>
       <c r="G4" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>C5,R1</v>
+        <v>C4,R0</v>
       </c>
       <c r="H4" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>C6,R1</v>
+        <v>C5,R0</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="12"/>
+      <c r="L4" s="10"/>
       <c r="P4" t="str">
         <f t="shared" ref="P4:T4" si="1">_xlfn.CONCAT(P3,",",$V$4)</f>
-        <v>C6,R1</v>
+        <v>C5,R0</v>
       </c>
       <c r="Q4" t="str">
         <f t="shared" si="1"/>
-        <v>C5,R1</v>
+        <v>C4,R0</v>
       </c>
       <c r="R4" t="str">
         <f t="shared" si="1"/>
-        <v>C4,R1</v>
+        <v>C3,R0</v>
       </c>
       <c r="S4" t="str">
         <f t="shared" si="1"/>
-        <v>C3,R1</v>
+        <v>C2,R0</v>
       </c>
       <c r="T4" t="str">
         <f t="shared" si="1"/>
-        <v>C2,R1</v>
+        <v>C1,R0</v>
       </c>
       <c r="U4" t="str">
         <f>_xlfn.CONCAT(U3,",",$V$4)</f>
-        <v>C1,R1</v>
-      </c>
-      <c r="V4" s="10" t="s">
-        <v>6</v>
+        <v>C0 ,R0</v>
+      </c>
+      <c r="V4" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="W4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>7</v>
+        <v>17</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>6</v>
       </c>
       <c r="C5" s="2" t="str">
         <f t="shared" ref="C5:H5" si="2">_xlfn.CONCAT(C3,",",$B$5)</f>
-        <v>C1,R2</v>
+        <v>C0,R1</v>
       </c>
       <c r="D5" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>C2,R2</v>
+        <v>C1,R1</v>
       </c>
       <c r="E5" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>C3,R2</v>
+        <v>C2,R1</v>
       </c>
       <c r="F5" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>C4,R2</v>
+        <v>C3,R1</v>
       </c>
       <c r="G5" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>C5,R2</v>
+        <v>C4,R1</v>
       </c>
       <c r="H5" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>C6,R2</v>
+        <v>C5,R1</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2" t="str">
         <f>_xlfn.CONCAT(K3,",",$B$5)</f>
-        <v>C9,R2</v>
-      </c>
-      <c r="L5" s="12"/>
+        <v>C8,R1</v>
+      </c>
+      <c r="L5" s="10"/>
       <c r="M5" t="str">
         <f t="shared" ref="M5:T5" si="3">_xlfn.CONCAT(M3,",",$V$5)</f>
-        <v>C9,R2</v>
+        <v>C8,R1</v>
       </c>
       <c r="P5" t="str">
         <f t="shared" si="3"/>
-        <v>C6,R2</v>
+        <v>C5,R1</v>
       </c>
       <c r="Q5" t="str">
         <f t="shared" si="3"/>
-        <v>C5,R2</v>
+        <v>C4,R1</v>
       </c>
       <c r="R5" t="str">
         <f t="shared" si="3"/>
-        <v>C4,R2</v>
+        <v>C3,R1</v>
       </c>
       <c r="S5" t="str">
         <f t="shared" si="3"/>
-        <v>C3,R2</v>
+        <v>C2,R1</v>
       </c>
       <c r="T5" t="str">
         <f t="shared" si="3"/>
-        <v>C2,R2</v>
+        <v>C1,R1</v>
       </c>
       <c r="U5" t="str">
         <f>_xlfn.CONCAT(U3,",",$V$5)</f>
-        <v>C1,R2</v>
-      </c>
-      <c r="V5" s="10" t="s">
-        <v>7</v>
+        <v>C0 ,R1</v>
+      </c>
+      <c r="V5" s="8" t="s">
+        <v>6</v>
       </c>
       <c r="W5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="C6" s="2" t="str">
         <f>_xlfn.CONCAT(C3,",",$B$6)</f>
-        <v>C1,R3</v>
+        <v>C0,R2</v>
       </c>
       <c r="D6" s="2" t="str">
         <f t="shared" ref="D6:K6" si="4">_xlfn.CONCAT(D3,",",$B$6)</f>
-        <v>C2,R3</v>
+        <v>C1,R2</v>
       </c>
       <c r="E6" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>C3,R3</v>
+        <v>C2,R2</v>
       </c>
       <c r="F6" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>C4,R3</v>
+        <v>C3,R2</v>
       </c>
       <c r="G6" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>C5,R3</v>
+        <v>C4,R2</v>
       </c>
       <c r="H6" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>C6,R3</v>
+        <v>C5,R2</v>
       </c>
       <c r="I6" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>C7,R3</v>
+        <v>C6,R2</v>
       </c>
       <c r="J6" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>C8,R3</v>
+        <v>C7,R2</v>
       </c>
       <c r="K6" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>C9,R3</v>
-      </c>
-      <c r="L6" s="12"/>
+        <v>C8,R2</v>
+      </c>
+      <c r="L6" s="10"/>
       <c r="M6" t="str">
         <f t="shared" ref="M6:T6" si="5">_xlfn.CONCAT(M3,",",$V$6)</f>
-        <v>C9,R3</v>
+        <v>C8,R2</v>
       </c>
       <c r="N6" t="str">
         <f t="shared" si="5"/>
-        <v>C8,R3</v>
+        <v>C7,R2</v>
       </c>
       <c r="O6" t="str">
         <f t="shared" si="5"/>
-        <v>C7,R3</v>
+        <v>C6,R2</v>
       </c>
       <c r="P6" t="str">
         <f t="shared" si="5"/>
-        <v>C6,R3</v>
+        <v>C5,R2</v>
       </c>
       <c r="Q6" t="str">
         <f t="shared" si="5"/>
-        <v>C5,R3</v>
+        <v>C4,R2</v>
       </c>
       <c r="R6" t="str">
         <f t="shared" si="5"/>
-        <v>C4,R3</v>
+        <v>C3,R2</v>
       </c>
       <c r="S6" t="str">
         <f t="shared" si="5"/>
-        <v>C3,R3</v>
+        <v>C2,R2</v>
       </c>
       <c r="T6" t="str">
         <f t="shared" si="5"/>
-        <v>C2,R3</v>
+        <v>C1,R2</v>
       </c>
       <c r="U6" t="str">
         <f>_xlfn.CONCAT(U3,",",$V$6)</f>
-        <v>C1,R3</v>
-      </c>
-      <c r="V6" s="10" t="s">
-        <v>8</v>
+        <v>C0 ,R2</v>
+      </c>
+      <c r="V6" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="W6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>9</v>
+        <v>18</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -980,34 +992,34 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2" t="str">
         <f>_xlfn.CONCAT(I3,",",$B$7)</f>
-        <v>C7,R4</v>
+        <v>C6,R3</v>
       </c>
       <c r="J7" s="2" t="str">
         <f>_xlfn.CONCAT(J3,",",$B$7)</f>
-        <v>C8,R4</v>
+        <v>C7,R3</v>
       </c>
       <c r="K7" s="2" t="str">
         <f>_xlfn.CONCAT(K3,",",$B$7)</f>
-        <v>C9,R4</v>
-      </c>
-      <c r="L7" s="12"/>
+        <v>C8,R3</v>
+      </c>
+      <c r="L7" s="10"/>
       <c r="M7" t="str">
         <f t="shared" ref="M7:O7" si="6">_xlfn.CONCAT(M3,",",$V$7)</f>
-        <v>C9,R4</v>
+        <v>C8,R3</v>
       </c>
       <c r="N7" t="str">
         <f t="shared" si="6"/>
-        <v>C8,R4</v>
+        <v>C7,R3</v>
       </c>
       <c r="O7" t="str">
         <f t="shared" si="6"/>
-        <v>C7,R4</v>
-      </c>
-      <c r="V7" s="10" t="s">
-        <v>9</v>
+        <v>C6,R3</v>
+      </c>
+      <c r="V7" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="W7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
@@ -1020,7 +1032,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="12"/>
+      <c r="L8" s="10"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C9" s="3">
@@ -1050,7 +1062,7 @@
       <c r="K9" s="4">
         <v>8</v>
       </c>
-      <c r="L9" s="12"/>
+      <c r="L9" s="10"/>
       <c r="M9" s="4">
         <v>8</v>
       </c>
@@ -1107,7 +1119,7 @@
       <c r="K10" s="3">
         <v>18</v>
       </c>
-      <c r="L10" s="12"/>
+      <c r="L10" s="10"/>
       <c r="M10" s="5">
         <v>18</v>
       </c>
@@ -1164,7 +1176,7 @@
       <c r="K11" s="3">
         <v>28</v>
       </c>
-      <c r="L11" s="12"/>
+      <c r="L11" s="10"/>
       <c r="M11" s="3">
         <v>28</v>
       </c>
@@ -1221,7 +1233,7 @@
       <c r="K12" s="3">
         <v>38</v>
       </c>
-      <c r="L12" s="12"/>
+      <c r="L12" s="10"/>
       <c r="M12" s="3">
         <v>38</v>
       </c>
@@ -1251,81 +1263,82 @@
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="L13" s="12"/>
+      <c r="L13" s="10"/>
+      <c r="O13" s="13"/>
     </row>
     <row r="14" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L14" s="12"/>
-      <c r="R14" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="S14" s="7"/>
-      <c r="T14" s="7"/>
-      <c r="U14" s="7"/>
+        <v>12</v>
+      </c>
+      <c r="L14" s="10"/>
+      <c r="R14" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="S14" s="11"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
       <c r="V14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="W14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L15" s="12"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
-      <c r="T15" s="7"/>
-      <c r="U15" s="7"/>
+        <v>11</v>
+      </c>
+      <c r="L15" s="10"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="11"/>
       <c r="V15" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="W15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
-      <c r="L16" s="12"/>
+      <c r="L16" s="10"/>
       <c r="V16" s="1"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L17" s="12"/>
+      <c r="L17" s="10"/>
       <c r="V17" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="W17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L18" s="12"/>
+        <v>29</v>
+      </c>
+      <c r="L18" s="10"/>
       <c r="V18" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="W18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>